<commit_message>
Buổi 11: thêm mới sản phẩm sử dụng react hook form
</commit_message>
<xml_diff>
--- a/diem_danh_giay_24_03_23_01_43_41.xlsx
+++ b/diem_danh_giay_24_03_23_01_43_41.xlsx
@@ -429,10 +429,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -469,13 +469,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -484,18 +477,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -507,9 +523,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -530,47 +545,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -598,16 +591,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -628,25 +628,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -659,12 +653,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,24 +676,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -718,7 +688,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -730,49 +772,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,25 +796,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,7 +850,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -859,7 +859,48 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -879,47 +920,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -931,148 +931,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1491,8 +1491,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1669,7 +1669,9 @@
       <c r="D6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>9</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1705,7 +1707,9 @@
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1741,7 +1745,9 @@
       <c r="D8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>9</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1777,7 +1783,9 @@
       <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>9</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1813,7 +1821,9 @@
       <c r="D10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>9</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1849,7 +1859,9 @@
       <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>9</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1885,7 +1897,9 @@
       <c r="D12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>9</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1921,7 +1935,9 @@
       <c r="D13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1">
+        <v>9</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1957,7 +1973,9 @@
       <c r="D14" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>9</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1993,7 +2011,9 @@
       <c r="D15" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>9</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -2029,7 +2049,9 @@
       <c r="D16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1">
+        <v>9</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -2065,7 +2087,9 @@
       <c r="D17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>9</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -2101,7 +2125,9 @@
       <c r="D18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>9</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2175,7 +2201,9 @@
       <c r="D20" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1">
+        <v>4</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -2211,7 +2239,9 @@
       <c r="D21" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1">
+        <v>9</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2247,7 +2277,9 @@
       <c r="D22" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1">
+        <v>9</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2283,7 +2315,9 @@
       <c r="D23" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1">
+        <v>9</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2319,7 +2353,9 @@
       <c r="D24" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1">
+        <v>9</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2393,7 +2429,9 @@
       <c r="D26" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1">
+        <v>9</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2429,7 +2467,9 @@
       <c r="D27" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>9</v>
+      </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2465,7 +2505,9 @@
       <c r="D28" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>9</v>
+      </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2501,7 +2543,9 @@
       <c r="D29" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="1">
+        <v>9</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2537,7 +2581,9 @@
       <c r="D30" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="1">
+        <v>9</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -2573,7 +2619,9 @@
       <c r="D31" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2609,7 +2657,9 @@
       <c r="D32" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>9</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2645,7 +2695,9 @@
       <c r="D33" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1">
+        <v>9</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2681,7 +2733,9 @@
       <c r="D34" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1">
+        <v>9</v>
+      </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2717,7 +2771,9 @@
       <c r="D35" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2753,7 +2809,9 @@
       <c r="D36" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1">
+        <v>9</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2789,7 +2847,9 @@
       <c r="D37" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2825,7 +2885,9 @@
       <c r="D38" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="1"/>
+      <c r="E38" s="1">
+        <v>9</v>
+      </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -2861,7 +2923,9 @@
       <c r="D39" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1">
+        <v>9</v>
+      </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -2897,7 +2961,9 @@
       <c r="D40" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1">
+        <v>9</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -2933,7 +2999,9 @@
       <c r="D41" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E41" s="1"/>
+      <c r="E41" s="1">
+        <v>9</v>
+      </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -2969,7 +3037,9 @@
       <c r="D42" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E42" s="1"/>
+      <c r="E42" s="1">
+        <v>9</v>
+      </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -3005,7 +3075,9 @@
       <c r="D43" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1">
+        <v>9</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -3041,7 +3113,9 @@
       <c r="D44" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="E44" s="1">
+        <v>9</v>
+      </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -3077,7 +3151,9 @@
       <c r="D45" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="E45" s="1"/>
+      <c r="E45" s="1">
+        <v>9</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>

</xml_diff>